<commit_message>
database config & doc update
</commit_message>
<xml_diff>
--- a/doc/计划.xlsx
+++ b/doc/计划.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01E125E-352F-4DCB-8A25-D91CD4CB8E63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D40590-CD77-498F-AB6E-B23B67CC3C90}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,51 +22,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
-    <t>汇报</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>//搬家
-修改设计</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>整理框架、建数据库</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>数据库设计、设计界面、制定计划</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>开发</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>调整进度
-开发</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>预期完成管理员端</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成公共组件
-预期完成各自第一个页面</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>调整进度
-预期完成3个页面</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>小学期</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>（视课程情况）完成学院端</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.完成公共组件（前端框架、Excel导入导出功能）
+2.预期完成各自第一个页面（数据库设计表1，表8）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>汇报进度，听取反馈</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.对已完成的代码进行必要修改
+2.预期完成3个页面（数据库设计表2、3、4，9、10、11）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>预期完成管理员端，择期交付展示</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.对已完成的代码进行必要修改
+2.继续完成其他页面</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.对已完成的代码进行必要修改
+2.继续完成其他页面</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>听取反馈，修改数据库设计、计划</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.整理学长框架，建立项目模板，在GitHub上建仓库
+2.完成数据库建立，完成数据字典表</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -157,40 +158,37 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -584,144 +582,147 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="31.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="31.21875" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3">
         <v>43686</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43687</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43688</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43689</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43690</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43691</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>0</v>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>43692</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>43693</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>43694</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>43695</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>0</v>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>43696</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>5</v>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>43697</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>43698</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>43699</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>43700</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>43701</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43702</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>10</v>
+      <c r="A18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>